<commit_message>
Ssit: update column J & Q
</commit_message>
<xml_diff>
--- a/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/ssit_vorlage.xlsx
+++ b/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/ssit_vorlage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ws-intern\PlanPro-Git\eclipse-set\java\bundles\org.eclipse.set.feature\rootdir\data\export\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9D10A7-DBB1-49B3-9201-F79FB7E379F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F503D209-483B-4B24-8E1A-A20D025FA2B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32760" yWindow="32760" windowWidth="28800" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -86,9 +86,6 @@
     <t>Taste</t>
   </si>
   <si>
-    <t>Anforderung NB</t>
-  </si>
-  <si>
     <t>Umstellung Weiche</t>
   </si>
   <si>
@@ -150,6 +147,9 @@
   <si>
     <t>Weichen-
 gruppe</t>
+  </si>
+  <si>
+    <t>Anforderung Nb</t>
   </si>
 </sst>
 </file>
@@ -990,7 +990,7 @@
   <dimension ref="A1:S61"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="115" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1052,22 +1052,22 @@
         <v>11</v>
       </c>
       <c r="N1" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="P1" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="P1" s="16" t="s">
-        <v>27</v>
-      </c>
       <c r="Q1" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="R1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="R1" s="16" t="s">
+      <c r="S1" s="16" t="s">
         <v>31</v>
-      </c>
-      <c r="S1" s="16" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1081,7 +1081,7 @@
       <c r="F2" s="35"/>
       <c r="G2" s="36"/>
       <c r="H2" s="34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I2" s="35"/>
       <c r="J2" s="35"/>
@@ -1100,16 +1100,16 @@
     <row r="3" spans="1:19" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F3" s="38"/>
       <c r="G3" s="39"/>
@@ -1123,7 +1123,7 @@
         <v>19</v>
       </c>
       <c r="K3" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L3" s="38"/>
       <c r="M3" s="38"/>
@@ -1140,7 +1140,7 @@
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>14</v>
@@ -1152,28 +1152,28 @@
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
       <c r="K4" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="N4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="N4" s="7" t="s">
+      <c r="O4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="O4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q4" s="10" t="s">
-        <v>22</v>
-      </c>
       <c r="R4" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S4" s="13"/>
     </row>
@@ -1196,7 +1196,7 @@
       <c r="P5" s="9"/>
       <c r="Q5" s="11"/>
       <c r="R5" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="S5" s="14"/>
     </row>
@@ -1470,6 +1470,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100E758A0F93049BE4CAD441F10C0D8186D" ma:contentTypeVersion="5" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="fb340e34ecc5d059b634082484788e96">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="576ce185-3b2e-4f75-8b7c-efeb82226bea" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v3/fields" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ae5cd419a40dc0c21009e0c04d2bd83e" ns2:_="" ns3:_="">
     <xsd:import namespace="576ce185-3b2e-4f75-8b7c-efeb82226bea"/>
@@ -1661,20 +1670,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -1720,7 +1716,19 @@
 </spe:Receivers>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF743650-405A-4EB5-9BE5-79180E38FBC9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B642628-E0AC-4F61-AC13-56E3126AE48A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1739,26 +1747,18 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF743650-405A-4EB5-9BE5-79180E38FBC9}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9CFCEAE-5A31-4E8D-871E-0FEB90E546B0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52AA9053-CA78-458B-BFEC-B0A103F9F68C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9CFCEAE-5A31-4E8D-871E-0FEB90E546B0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Ssit: update column J & Q (#1368)
</commit_message>
<xml_diff>
--- a/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/ssit_vorlage.xlsx
+++ b/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/ssit_vorlage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ws-intern\PlanPro-Git\eclipse-set\java\bundles\org.eclipse.set.feature\rootdir\data\export\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9D10A7-DBB1-49B3-9201-F79FB7E379F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F503D209-483B-4B24-8E1A-A20D025FA2B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32760" yWindow="32760" windowWidth="28800" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -86,9 +86,6 @@
     <t>Taste</t>
   </si>
   <si>
-    <t>Anforderung NB</t>
-  </si>
-  <si>
     <t>Umstellung Weiche</t>
   </si>
   <si>
@@ -150,6 +147,9 @@
   <si>
     <t>Weichen-
 gruppe</t>
+  </si>
+  <si>
+    <t>Anforderung Nb</t>
   </si>
 </sst>
 </file>
@@ -990,7 +990,7 @@
   <dimension ref="A1:S61"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="115" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1052,22 +1052,22 @@
         <v>11</v>
       </c>
       <c r="N1" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="P1" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="P1" s="16" t="s">
-        <v>27</v>
-      </c>
       <c r="Q1" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="R1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="R1" s="16" t="s">
+      <c r="S1" s="16" t="s">
         <v>31</v>
-      </c>
-      <c r="S1" s="16" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1081,7 +1081,7 @@
       <c r="F2" s="35"/>
       <c r="G2" s="36"/>
       <c r="H2" s="34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I2" s="35"/>
       <c r="J2" s="35"/>
@@ -1100,16 +1100,16 @@
     <row r="3" spans="1:19" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F3" s="38"/>
       <c r="G3" s="39"/>
@@ -1123,7 +1123,7 @@
         <v>19</v>
       </c>
       <c r="K3" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L3" s="38"/>
       <c r="M3" s="38"/>
@@ -1140,7 +1140,7 @@
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>14</v>
@@ -1152,28 +1152,28 @@
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
       <c r="K4" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="N4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="N4" s="7" t="s">
+      <c r="O4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="O4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q4" s="10" t="s">
-        <v>22</v>
-      </c>
       <c r="R4" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S4" s="13"/>
     </row>
@@ -1196,7 +1196,7 @@
       <c r="P5" s="9"/>
       <c r="Q5" s="11"/>
       <c r="R5" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="S5" s="14"/>
     </row>
@@ -1470,6 +1470,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100E758A0F93049BE4CAD441F10C0D8186D" ma:contentTypeVersion="5" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="fb340e34ecc5d059b634082484788e96">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="576ce185-3b2e-4f75-8b7c-efeb82226bea" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v3/fields" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ae5cd419a40dc0c21009e0c04d2bd83e" ns2:_="" ns3:_="">
     <xsd:import namespace="576ce185-3b2e-4f75-8b7c-efeb82226bea"/>
@@ -1661,20 +1670,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -1720,7 +1716,19 @@
 </spe:Receivers>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF743650-405A-4EB5-9BE5-79180E38FBC9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B642628-E0AC-4F61-AC13-56E3126AE48A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1739,26 +1747,18 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF743650-405A-4EB5-9BE5-79180E38FBC9}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9CFCEAE-5A31-4E8D-871E-0FEB90E546B0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52AA9053-CA78-458B-BFEC-B0A103F9F68C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9CFCEAE-5A31-4E8D-871E-0FEB90E546B0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>